<commit_message>
Fix error in computing number of failing scenarios
In addition, add a row to features_vs_specifications.xlsx indicating, for each specification, if ATGT should be able to generate a test suite or not.
</commit_message>
<xml_diff>
--- a/code/experimental/asmeta.evotest/asmeta.evotest.experiments/features_vs_specifications.xlsx
+++ b/code/experimental/asmeta.evotest/asmeta.evotest.experiments/features_vs_specifications.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nico.pellegrinelli\Desktop\RepoLocaliGit\asmeta\code\experimental\asmeta.evotest\asmeta.evotest.experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20596DD3-4954-45AA-8796-93A5A4BE6CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6294B72D-4601-416E-85B6-8E77949DE7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="57">
   <si>
     <t>FEATURES</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>with rule as term</t>
+  </si>
+  <si>
+    <t>SHOULD ATGT BE ABLE TO GENERATE TESTS?</t>
   </si>
 </sst>
 </file>
@@ -289,7 +292,117 @@
     <cellStyle name="Migliaia" xfId="1" builtinId="3"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -606,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W33"/>
+  <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,15 +1385,100 @@
         <v>Yes</v>
       </c>
     </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" t="str">
+        <f>IF(COUNTIFS(C3:C33,"X",B3:B33,"No")&gt;0,"No","Yes")</f>
+        <v>Yes</v>
+      </c>
+      <c r="D35" t="str">
+        <f>IF(COUNTIFS(D3:D33,"X",B3:B33,"No")&gt;0,"No","Yes")</f>
+        <v>No</v>
+      </c>
+      <c r="E35" t="str">
+        <f>IF(COUNTIFS(E3:E33,"X",B3:B33,"No")&gt;0,"No","Yes")</f>
+        <v>No</v>
+      </c>
+      <c r="F35" t="str">
+        <f>IF(COUNTIFS(F3:F33,"X",B3:B33,"No")&gt;0,"No","Yes")</f>
+        <v>Yes</v>
+      </c>
+      <c r="G35" t="str">
+        <f>IF(COUNTIFS(G3:G33,"X",B3:B33,"No")&gt;0,"No","Yes")</f>
+        <v>Yes</v>
+      </c>
+      <c r="H35" t="str">
+        <f>IF(COUNTIFS(H3:H33,"X",B3:B33,"No")&gt;0,"No","Yes")</f>
+        <v>Yes</v>
+      </c>
+      <c r="I35" t="str">
+        <f>IF(COUNTIFS(I3:I33,"X",B3:B33,"No")&gt;0,"No","Yes")</f>
+        <v>No</v>
+      </c>
+      <c r="J35" t="str">
+        <f>IF(COUNTIFS(J3:J33,"X",B3:B33,"No")&gt;0,"No","Yes")</f>
+        <v>No</v>
+      </c>
+      <c r="K35" t="str">
+        <f>IF(COUNTIFS(K3:K33,"X",B3:B33,"No")&gt;0,"No","Yes")</f>
+        <v>Yes</v>
+      </c>
+      <c r="L35" t="str">
+        <f>IF(COUNTIFS(L3:L33,"X",B3:B33,"No")&gt;0,"No","Yes")</f>
+        <v>Yes</v>
+      </c>
+      <c r="M35" t="str">
+        <f>IF(COUNTIFS(M3:M33,"X",B3:B33,"No")&gt;0,"No","Yes")</f>
+        <v>No</v>
+      </c>
+      <c r="N35" t="str">
+        <f>IF(COUNTIFS(N3:N33,"X",B3:B33,"No")&gt;0,"No","Yes")</f>
+        <v>Yes</v>
+      </c>
+      <c r="O35" t="str">
+        <f>IF(COUNTIFS(O3:O33,"X",B3:B33,"No")&gt;0,"No","Yes")</f>
+        <v>Yes</v>
+      </c>
+      <c r="P35" t="str">
+        <f>IF(COUNTIFS(P3:P33,"X",B3:B33,"No")&gt;0,"No","Yes")</f>
+        <v>No</v>
+      </c>
+      <c r="Q35" t="str">
+        <f>IF(COUNTIFS(Q3:Q33,"X",B3:B33,"No")&gt;0,"No","Yes")</f>
+        <v>No</v>
+      </c>
+      <c r="R35" t="str">
+        <f>IF(COUNTIFS(R3:R33,"X",B3:B33,"No")&gt;0,"No","Yes")</f>
+        <v>No</v>
+      </c>
+      <c r="S35" t="str">
+        <f>IF(COUNTIFS(S3:S33,"X",B3:B33,"No")&gt;0,"No","Yes")</f>
+        <v>Yes</v>
+      </c>
+      <c r="T35" t="str">
+        <f>IF(COUNTIFS(T3:T33,"X",B3:B33,"No")&gt;0,"No","Yes")</f>
+        <v>No</v>
+      </c>
+      <c r="U35" t="str">
+        <f>IF(COUNTIFS(U3:U33,"X",B3:B33,"No")&gt;0,"No","Yes")</f>
+        <v>Yes</v>
+      </c>
+      <c r="V35" t="str">
+        <f>IF(COUNTIFS(V3:V33,"X",B3:B33,"No")&gt;0,"No","Yes")</f>
+        <v>No</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A21">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="iconSet" priority="3">
+    <cfRule type="iconSet" priority="5">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1289,15 +1487,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B19 B21:B32 B34">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B19 B21:B32">
-    <cfRule type="iconSet" priority="24">
+    <cfRule type="iconSet" priority="26">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1305,6 +1503,14 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C35:V35">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>